<commit_message>
final commit, written README, refactored config
</commit_message>
<xml_diff>
--- a/result/times_and_diagram.xlsx
+++ b/result/times_and_diagram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pyProjects\Lab3DB\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lab3_database_benchmark\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D167203C-A1CE-40D0-B5D5-61990DE3A701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47064693-BDC9-4BE7-A040-00CAF6468453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6FA6A41B-C630-4ACE-9274-5E3827EC49F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{6FA6A41B-C630-4ACE-9274-5E3827EC49F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>1 query</t>
   </si>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +70,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -117,11 +125,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -174,11 +185,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average times</a:t>
+              <a:t>Average times between Psycopg2,</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> between different libraries</a:t>
+              <a:t> Pandas, SQLAlchemy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -215,17 +230,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.4015322244626733E-2"/>
-          <c:y val="0.10463474524248007"/>
-          <c:w val="0.93246594465378962"/>
-          <c:h val="0.74474098886810425"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -235,11 +240,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$2</c:f>
+              <c:f>Лист1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1 query</c:v>
+                  <c:v>Psycopg2 (tiny)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -256,54 +261,48 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$B$1:$F$1</c:f>
+              <c:f>Лист1!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Psycopg2 (tiny)</c:v>
+                  <c:v>1 query</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQLite3 (big)</c:v>
+                  <c:v>2 query</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Pandas (tiny)</c:v>
+                  <c:v>3 query</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SQLAlchemy (tiny)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DuckDB (big)</c:v>
+                  <c:v>4 query</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$F$2</c:f>
+              <c:f>Лист1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.31162624000000899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9896814299999903</c:v>
+                  <c:v>0.37879921499999197</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29983326999993098</c:v>
+                  <c:v>1.1999884399999901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.260730289999969</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2604190549999801</c:v>
+                  <c:v>1.48664225999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-17F7-4307-AEB3-679CE2232B30}"/>
+              <c16:uniqueId val="{00000000-BBF8-4E3C-87D2-298F74548282}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -312,11 +311,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$3</c:f>
+              <c:f>Лист1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 query</c:v>
+                  <c:v>Pandas (tiny)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -333,54 +332,48 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$B$1:$F$1</c:f>
+              <c:f>Лист1!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Psycopg2 (tiny)</c:v>
+                  <c:v>1 query</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQLite3 (big)</c:v>
+                  <c:v>2 query</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Pandas (tiny)</c:v>
+                  <c:v>3 query</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SQLAlchemy (tiny)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DuckDB (big)</c:v>
+                  <c:v>4 query</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$3:$F$3</c:f>
+              <c:f>Лист1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.37879921499999197</c:v>
+                  <c:v>0.29983326999993098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.886131945000001</c:v>
+                  <c:v>0.38601846499996101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38601846499996101</c:v>
+                  <c:v>1.16808098500005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37843343499987397</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.50587303999998</c:v>
+                  <c:v>1.4567115949999501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-17F7-4307-AEB3-679CE2232B30}"/>
+              <c16:uniqueId val="{00000001-BBF8-4E3C-87D2-298F74548282}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -389,11 +382,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$4</c:f>
+              <c:f>Лист1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3 query</c:v>
+                  <c:v>SQLAlchemy (tiny)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -410,131 +403,48 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$B$1:$F$1</c:f>
+              <c:f>Лист1!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Psycopg2 (tiny)</c:v>
+                  <c:v>1 query</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQLite3 (big)</c:v>
+                  <c:v>2 query</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Pandas (tiny)</c:v>
+                  <c:v>3 query</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SQLAlchemy (tiny)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DuckDB (big)</c:v>
+                  <c:v>4 query</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$4:$F$4</c:f>
+              <c:f>Лист1!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.1999884399999901</c:v>
+                  <c:v>0.260730289999969</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.3215607449999</c:v>
+                  <c:v>0.37843343499987397</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.16808098500005</c:v>
+                  <c:v>1.14467158000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.14467158000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7701316500000299</c:v>
+                  <c:v>1.45481115999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-17F7-4307-AEB3-679CE2232B30}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4 query</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Лист1!$B$1:$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Psycopg2 (tiny)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SQLite3 (big)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Pandas (tiny)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>SQLAlchemy (tiny)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>DuckDB (big)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$B$5:$F$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.48664225999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40.392246099999902</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4567115949999501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.45481115999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.09123613499998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-17F7-4307-AEB3-679CE2232B30}"/>
+              <c16:uniqueId val="{00000002-BBF8-4E3C-87D2-298F74548282}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -548,16 +458,72 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="366991599"/>
-        <c:axId val="370449551"/>
+        <c:axId val="457256352"/>
+        <c:axId val="257383104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="366991599"/>
+        <c:axId val="457256352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Modules</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU" sz="1200" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -580,7 +546,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -595,7 +561,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370449551"/>
+        <c:crossAx val="257383104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -603,7 +569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="370449551"/>
+        <c:axId val="257383104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,6 +589,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU" sz="1200" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6494845360824743E-2"/>
+              <c:y val="0.32745073022077958"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -639,7 +669,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -654,7 +684,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366991599"/>
+        <c:crossAx val="457256352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -681,7 +711,563 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Average times between SQLite3, DuckDB</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SQLite3 (big)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$G$2:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1 query</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 query</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 query</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 query</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.9896814299999903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.886131945000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.3215607449999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.392246099999902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B6F3-4EBC-9207-845F54B20264}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DuckDB (big)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$G$2:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1 query</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 query</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 query</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 query</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$I$2:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.2604190549999801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.50587303999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7701316500000299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.09123613499998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B6F3-4EBC-9207-845F54B20264}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="263719712"/>
+        <c:axId val="265892080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="263719712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Modules</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265892080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="265892080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7121455323702513E-2"/>
+              <c:y val="0.32826746603652274"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="263719712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -781,6 +1367,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1284,27 +1910,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1287780</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Диаграмма 2">
+        <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0886FB22-96CB-BF5C-5E7C-CFEC91F3A7A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEC48105-45B9-25C8-62F5-7BCC8B04D2FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1317,6 +2446,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>473074</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>577849</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43104A61-2700-B9A7-C7A8-568F83084E94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1622,40 +2787,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B285823D-E81D-4050-980E-FD55BA387975}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1663,19 +2832,22 @@
         <v>0.31162624000000899</v>
       </c>
       <c r="C2" s="1">
+        <v>0.29983326999993098</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.260730289999969</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
         <v>5.9896814299999903</v>
       </c>
-      <c r="D2" s="1">
-        <v>0.29983326999993098</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.260730289999969</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="I2" s="1">
         <v>1.2604190549999801</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1683,19 +2855,22 @@
         <v>0.37879921499999197</v>
       </c>
       <c r="C3" s="1">
+        <v>0.38601846499996101</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.37843343499987397</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>10.886131945000001</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.38601846499996101</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.37843343499987397</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="I3" s="1">
         <v>1.50587303999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1703,19 +2878,22 @@
         <v>1.1999884399999901</v>
       </c>
       <c r="C4" s="1">
+        <v>1.16808098500005</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.14467158000002</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
         <v>18.3215607449999</v>
       </c>
-      <c r="D4" s="1">
-        <v>1.16808098500005</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.14467158000002</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="I4" s="1">
         <v>1.7701316500000299</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1723,17 +2901,23 @@
         <v>1.48664225999999</v>
       </c>
       <c r="C5" s="1">
+        <v>1.4567115949999501</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.45481115999998</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
         <v>40.392246099999902</v>
       </c>
-      <c r="D5" s="1">
-        <v>1.4567115949999501</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.45481115999998</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="I5" s="1">
         <v>2.09123613499998</v>
       </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="G10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>